<commit_message>
Atualiza FUNC.xlsx com dados mais recentes
- Atualizado do Google Drive: projeto_atendimento/NIBO WEB API/
- Total de funcionários: 158 (eram 156)
- Estrutura mantida: matricula, nome, Coluna2 (StakeholderID)
- Novos funcionários adicionados
</commit_message>
<xml_diff>
--- a/projeto/FUNC.xlsx
+++ b/projeto/FUNC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\projeto_atendimento\NIBO WEB API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84C601A-CD27-482D-B324-482DDB4D75C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6664AC-8482-4FAA-9513-243A7708758E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13335" xr2:uid="{A5566D1E-FB50-4646-A727-6AF21217A2FB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="316">
   <si>
     <t>nome</t>
   </si>
@@ -975,19 +975,34 @@
   </si>
   <si>
     <t>33fe4e6f-e22a-45c7-b162-1e031ee3cc71</t>
+  </si>
+  <si>
+    <t>a8fc-4770-968d-93cc49ced1bd</t>
+  </si>
+  <si>
+    <t>PALOMA DE JESUS SANTOS</t>
+  </si>
+  <si>
+    <t>29b41aac-c42c-4190-8652-60e5410b593a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF5A5C5E"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1016,9 +1031,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1355,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26FDFC0-3A15-4C58-8EAD-DAE315CBFD7D}">
-  <dimension ref="A1:C157"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+      <selection activeCell="B164" sqref="B164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3093,10 +3111,33 @@
         <v>312</v>
       </c>
     </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A158">
+        <v>5283</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C158" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A159">
+        <v>5284</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C159" t="s">
+        <v>315</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C156">
     <sortCondition ref="B1:B156"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>